<commit_message>
Commercial Studies Courses Fixed
</commit_message>
<xml_diff>
--- a/Offline/TeacherRecruitment/Teacher Payment Slabs.xlsx
+++ b/Offline/TeacherRecruitment/Teacher Payment Slabs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5850" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5856" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="49">
   <si>
     <t>Physics</t>
   </si>
@@ -173,6 +173,9 @@
   <si>
     <t>ICSE / CBSE VIII</t>
   </si>
+  <si>
+    <t>&gt; 40</t>
+  </si>
 </sst>
 </file>
 
@@ -593,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -682,34 +685,10 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -738,6 +717,33 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1075,15 +1081,15 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="3.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -1092,7 +1098,7 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1101,7 +1107,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1110,7 +1116,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -1119,7 +1125,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -1128,7 +1134,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1137,7 +1143,7 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -1146,7 +1152,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -1155,18 +1161,18 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="2:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -1175,7 +1181,7 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -1184,29 +1190,29 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -1215,18 +1221,18 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -1235,18 +1241,18 @@
       <c r="G17" s="8"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="7"/>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -1276,300 +1282,300 @@
   </sheetPr>
   <dimension ref="B1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:D31"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="22.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="1"/>
-    <col min="2" max="2" width="43.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="22.42578125" style="1"/>
+    <col min="1" max="1" width="22.44140625" style="1"/>
+    <col min="2" max="2" width="43.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="22.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="42" t="s">
+    <row r="1" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" ht="24.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="36" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="35" t="s">
+    <row r="3" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B3" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="36">
+      <c r="D3" s="30">
         <v>36000</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-      <c r="C4" s="45" t="s">
+    <row r="4" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B4" s="44"/>
+      <c r="C4" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="30">
         <v>36000</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="37"/>
-      <c r="C5" s="46" t="s">
+    <row r="5" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B5" s="44"/>
+      <c r="C5" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="31">
         <v>28000</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="37"/>
-      <c r="C6" s="46" t="s">
+    <row r="6" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B6" s="44"/>
+      <c r="C6" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="31">
         <v>24000</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="37"/>
-      <c r="C7" s="46" t="s">
+    <row r="7" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B7" s="44"/>
+      <c r="C7" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="31">
         <v>24000</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="37"/>
-      <c r="C8" s="46" t="s">
+    <row r="8" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B8" s="44"/>
+      <c r="C8" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="31">
         <v>20000</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="37"/>
-      <c r="C9" s="46" t="s">
+    <row r="9" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B9" s="44"/>
+      <c r="C9" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="31">
         <v>20000</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="39"/>
-      <c r="C10" s="47" t="s">
+    <row r="10" spans="2:4" ht="19.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="45"/>
+      <c r="C10" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="32">
         <v>18000</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="35" t="s">
+    <row r="11" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B11" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="41">
+      <c r="D11" s="33">
         <v>18000</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="37"/>
-      <c r="C12" s="46" t="s">
+    <row r="12" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B12" s="44"/>
+      <c r="C12" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="31">
         <v>14000</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="37"/>
-      <c r="C13" s="46" t="s">
+    <row r="13" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B13" s="44"/>
+      <c r="C13" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="31">
         <v>12000</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="37"/>
-      <c r="C14" s="46" t="s">
+    <row r="14" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B14" s="44"/>
+      <c r="C14" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="38">
+      <c r="D14" s="31">
         <v>12000</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
-      <c r="C15" s="46" t="s">
+    <row r="15" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B15" s="44"/>
+      <c r="C15" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="38">
+      <c r="D15" s="31">
         <v>10000</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="37"/>
-      <c r="C16" s="46" t="s">
+    <row r="16" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B16" s="44"/>
+      <c r="C16" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="38">
+      <c r="D16" s="31">
         <v>10000</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="39"/>
-      <c r="C17" s="47" t="s">
+    <row r="17" spans="2:4" ht="19.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="45"/>
+      <c r="C17" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="40">
+      <c r="D17" s="32">
         <v>9000</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B18" s="35" t="s">
+    <row r="18" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B18" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="41">
+      <c r="D18" s="33">
         <v>9000</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="37"/>
-      <c r="C19" s="46" t="s">
+    <row r="19" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B19" s="44"/>
+      <c r="C19" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="38">
+      <c r="D19" s="31">
         <v>7000</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="37"/>
-      <c r="C20" s="46" t="s">
+    <row r="20" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B20" s="44"/>
+      <c r="C20" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="38">
+      <c r="D20" s="31">
         <v>6000</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="37"/>
-      <c r="C21" s="46" t="s">
+    <row r="21" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B21" s="44"/>
+      <c r="C21" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="38">
+      <c r="D21" s="31">
         <v>6000</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B22" s="37"/>
-      <c r="C22" s="46" t="s">
+    <row r="22" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B22" s="44"/>
+      <c r="C22" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="38">
+      <c r="D22" s="31">
         <v>5000</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="37"/>
-      <c r="C23" s="46" t="s">
+    <row r="23" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B23" s="44"/>
+      <c r="C23" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="38">
+      <c r="D23" s="31">
         <v>5000</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="39"/>
-      <c r="C24" s="47" t="s">
+    <row r="24" spans="2:4" ht="19.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="45"/>
+      <c r="C24" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="40">
+      <c r="D24" s="32">
         <v>4500</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B25" s="35" t="s">
+    <row r="25" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B25" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="48" t="s">
+      <c r="C25" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="41">
+      <c r="D25" s="33">
         <v>4500</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B26" s="37"/>
-      <c r="C26" s="46" t="s">
+    <row r="26" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B26" s="44"/>
+      <c r="C26" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="38">
+      <c r="D26" s="31">
         <v>3500</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="37"/>
-      <c r="C27" s="46" t="s">
+    <row r="27" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B27" s="44"/>
+      <c r="C27" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="38">
+      <c r="D27" s="31">
         <v>3000</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="37"/>
-      <c r="C28" s="46" t="s">
+    <row r="28" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B28" s="44"/>
+      <c r="C28" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="38">
+      <c r="D28" s="31">
         <v>3000</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B29" s="37"/>
-      <c r="C29" s="46" t="s">
+    <row r="29" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B29" s="44"/>
+      <c r="C29" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="38">
+      <c r="D29" s="31">
         <v>2500</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B30" s="37"/>
-      <c r="C30" s="46" t="s">
+    <row r="30" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.25">
+      <c r="B30" s="44"/>
+      <c r="C30" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="38">
+      <c r="D30" s="31">
         <v>2500</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="39"/>
-      <c r="C31" s="47" t="s">
+    <row r="31" spans="2:4" ht="19.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="45"/>
+      <c r="C31" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="40">
+      <c r="D31" s="32">
         <v>2250</v>
       </c>
     </row>
@@ -1590,39 +1596,39 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:S47"/>
+  <dimension ref="B1:V47"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3:S3"/>
+      <selection pane="bottomRight" activeCell="V3" sqref="V3:V52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1"/>
-    <col min="2" max="2" width="17.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="1"/>
+    <col min="2" max="2" width="17.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="14.7109375" style="1"/>
+    <col min="14" max="14" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="14.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:19" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:19" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>25</v>
       </c>
@@ -1678,27 +1684,27 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="32" t="s">
+    <row r="3" spans="2:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="34"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="48"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
@@ -2134,7 +2140,7 @@
       <c r="R13" s="17"/>
       <c r="S13" s="18"/>
     </row>
-    <row r="14" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="20"/>
       <c r="C14" s="21" t="s">
         <v>24</v>
@@ -2610,7 +2616,7 @@
       <c r="R24" s="17"/>
       <c r="S24" s="18"/>
     </row>
-    <row r="25" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="20"/>
       <c r="C25" s="21" t="s">
         <v>24</v>
@@ -2960,7 +2966,7 @@
       <c r="R32" s="17"/>
       <c r="S32" s="18"/>
     </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B33" s="14"/>
       <c r="C33" s="15" t="s">
         <v>20</v>
@@ -3002,7 +3008,7 @@
       <c r="R33" s="17"/>
       <c r="S33" s="18"/>
     </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B34" s="14"/>
       <c r="C34" s="15" t="s">
         <v>22</v>
@@ -3044,7 +3050,7 @@
       <c r="R34" s="17"/>
       <c r="S34" s="18"/>
     </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B35" s="14"/>
       <c r="C35" s="15" t="s">
         <v>23</v>
@@ -3086,7 +3092,7 @@
       <c r="R35" s="17"/>
       <c r="S35" s="18"/>
     </row>
-    <row r="36" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:22" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="20"/>
       <c r="C36" s="21" t="s">
         <v>24</v>
@@ -3128,9 +3134,9 @@
       <c r="R36" s="23"/>
       <c r="S36" s="24"/>
     </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B37" s="9" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>14</v>
@@ -3158,7 +3164,7 @@
       <c r="R37" s="11"/>
       <c r="S37" s="13"/>
     </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B38" s="14"/>
       <c r="C38" s="15" t="s">
         <v>15</v>
@@ -3186,7 +3192,7 @@
       <c r="R38" s="17"/>
       <c r="S38" s="18"/>
     </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B39" s="14"/>
       <c r="C39" s="15" t="s">
         <v>16</v>
@@ -3240,7 +3246,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="40" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B40" s="14"/>
       <c r="C40" s="15" t="s">
         <v>17</v>
@@ -3293,8 +3299,9 @@
       <c r="S40" s="19">
         <v>18000</v>
       </c>
-    </row>
-    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V40" s="49"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B41" s="14"/>
       <c r="C41" s="15" t="s">
         <v>18</v>
@@ -3348,7 +3355,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B42" s="14"/>
       <c r="C42" s="15" t="s">
         <v>21</v>
@@ -3392,7 +3399,7 @@
       <c r="R42" s="17"/>
       <c r="S42" s="18"/>
     </row>
-    <row r="43" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B43" s="14"/>
       <c r="C43" s="15" t="s">
         <v>19</v>
@@ -3436,7 +3443,7 @@
       <c r="R43" s="17"/>
       <c r="S43" s="18"/>
     </row>
-    <row r="44" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B44" s="14"/>
       <c r="C44" s="15" t="s">
         <v>20</v>
@@ -3478,7 +3485,7 @@
       <c r="R44" s="17"/>
       <c r="S44" s="18"/>
     </row>
-    <row r="45" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B45" s="14"/>
       <c r="C45" s="15" t="s">
         <v>22</v>
@@ -3520,7 +3527,7 @@
       <c r="R45" s="17"/>
       <c r="S45" s="18"/>
     </row>
-    <row r="46" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B46" s="14"/>
       <c r="C46" s="15" t="s">
         <v>23</v>
@@ -3562,7 +3569,7 @@
       <c r="R46" s="17"/>
       <c r="S46" s="18"/>
     </row>
-    <row r="47" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:22" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="20"/>
       <c r="C47" s="21" t="s">
         <v>24</v>
@@ -3627,30 +3634,30 @@
       <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="1"/>
-    <col min="2" max="2" width="17.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="12" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="2:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:19" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="25" t="s">
         <v>32</v>
@@ -3673,7 +3680,7 @@
       <c r="R2" s="26"/>
       <c r="S2" s="27"/>
     </row>
-    <row r="3" spans="2:19" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:19" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>25</v>
       </c>
@@ -4185,7 +4192,7 @@
       <c r="R14" s="17"/>
       <c r="S14" s="18"/>
     </row>
-    <row r="15" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="20"/>
       <c r="C15" s="21" t="s">
         <v>24</v>
@@ -4661,7 +4668,7 @@
       <c r="R25" s="17"/>
       <c r="S25" s="18"/>
     </row>
-    <row r="26" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="20"/>
       <c r="C26" s="21" t="s">
         <v>24</v>
@@ -5137,7 +5144,7 @@
       <c r="R36" s="17"/>
       <c r="S36" s="18"/>
     </row>
-    <row r="37" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="20"/>
       <c r="C37" s="21" t="s">
         <v>24</v>
@@ -5613,7 +5620,7 @@
       <c r="R47" s="17"/>
       <c r="S47" s="18"/>
     </row>
-    <row r="48" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="20"/>
       <c r="C48" s="21" t="s">
         <v>24</v>

</xml_diff>